<commit_message>
search input value divde inot 3 func: 1. check format 2. check value 2.1 check single value with related rule
</commit_message>
<xml_diff>
--- a/doc/error_code_range.xlsx
+++ b/doc/error_code_range.xlsx
@@ -1,10 +1,10 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="3" lowestEdited="5" rupBuild="9302"/>
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
   <workbookPr/>
   <bookViews>
-    <workbookView windowWidth="28695" windowHeight="13050"/>
+    <workbookView xWindow="0" yWindow="60" windowWidth="28695" windowHeight="12990"/>
   </bookViews>
   <sheets>
     <sheet name="all" sheetId="1" r:id="rId1"/>
@@ -172,7 +172,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="F18" authorId="1">
+    <comment ref="F19" authorId="1">
       <text>
         <r>
           <rPr>
@@ -185,7 +185,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="F19" authorId="1">
+    <comment ref="F20" authorId="1">
       <text>
         <r>
           <rPr>
@@ -203,31 +203,31 @@
             <charset val="134"/>
           </rPr>
           <t>虽然在misc中，但是是个大函数，所以有单独的error code范围</t>
-        </r>
-      </text>
-    </comment>
-    <comment ref="A22" authorId="0">
-      <text>
-        <r>
-          <rPr>
-            <sz val="9"/>
-            <rFont val="宋体"/>
-            <charset val="134"/>
-          </rPr>
-          <t xml:space="preserve">zw:
-</t>
-        </r>
-        <r>
-          <rPr>
-            <sz val="9"/>
-            <rFont val="宋体"/>
-            <charset val="134"/>
-          </rPr>
-          <t>全局配置以及对应的错误</t>
         </r>
       </text>
     </comment>
     <comment ref="A23" authorId="0">
+      <text>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <rFont val="宋体"/>
+            <charset val="134"/>
+          </rPr>
+          <t xml:space="preserve">zw:
+</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <rFont val="宋体"/>
+            <charset val="134"/>
+          </rPr>
+          <t>全局配置以及对应的错误</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="A24" authorId="0">
       <text>
         <r>
           <rPr>
@@ -253,7 +253,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="40">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="42" uniqueCount="42">
   <si>
     <t>rc</t>
   </si>
@@ -388,9 +388,6 @@
     <t>69800-69899</t>
   </si>
   <si>
-    <t>validateInputRule</t>
-  </si>
-  <si>
     <r>
       <rPr>
         <sz val="11"/>
@@ -425,18 +422,24 @@
   <si>
     <t>uploadDefine</t>
   </si>
+  <si>
+    <t>69500-69599</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>validateInputRule</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>validateInputSearch</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <numFmts count="4">
-    <numFmt numFmtId="44" formatCode="_ &quot;￥&quot;* #,##0.00_ ;_ &quot;￥&quot;* \-#,##0.00_ ;_ &quot;￥&quot;* &quot;-&quot;??_ ;_ @_ "/>
-    <numFmt numFmtId="41" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
-    <numFmt numFmtId="43" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
-    <numFmt numFmtId="42" formatCode="_ &quot;￥&quot;* #,##0_ ;_ &quot;￥&quot;* \-#,##0_ ;_ &quot;￥&quot;* &quot;-&quot;_ ;_ @_ "/>
-  </numFmts>
-  <fonts count="22">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color indexed="8"/>
@@ -451,352 +454,20 @@
       <charset val="134"/>
     </font>
     <font>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FFFFFFFF"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="13"/>
-      <color theme="3"/>
+      <sz val="9"/>
       <name val="宋体"/>
       <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FFFF0000"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="宋体"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <i/>
-      <sz val="11"/>
-      <color rgb="FF7F7F7F"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color theme="3"/>
-      <name val="宋体"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <u/>
-      <sz val="11"/>
-      <color rgb="FF800080"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF9C0006"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color theme="0"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FF3F3F3F"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="15"/>
-      <color theme="3"/>
-      <name val="宋体"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="18"/>
-      <color theme="3"/>
-      <name val="宋体"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <u/>
-      <sz val="11"/>
-      <color rgb="FF0000FF"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF9C6500"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF3F3F76"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FFFA7D00"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FFFA7D00"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF006100"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="33">
+  <fills count="2">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
     </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFA5A5A5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFC7CE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFF2F2F2"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFFFCC"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFEB9C"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFCC99"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFC6EFCE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
   </fills>
-  <borders count="9">
+  <borders count="1">
     <border>
       <left/>
       <right/>
@@ -804,251 +475,9 @@
       <bottom/>
       <diagonal/>
     </border>
-    <border>
-      <left style="double">
-        <color rgb="FF3F3F3F"/>
-      </left>
-      <right style="double">
-        <color rgb="FF3F3F3F"/>
-      </right>
-      <top style="double">
-        <color rgb="FF3F3F3F"/>
-      </top>
-      <bottom style="double">
-        <color rgb="FF3F3F3F"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="medium">
-        <color theme="4"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color rgb="FF3F3F3F"/>
-      </left>
-      <right style="thin">
-        <color rgb="FF3F3F3F"/>
-      </right>
-      <top style="thin">
-        <color rgb="FF3F3F3F"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FF3F3F3F"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color rgb="FFB2B2B2"/>
-      </left>
-      <right style="thin">
-        <color rgb="FFB2B2B2"/>
-      </right>
-      <top style="thin">
-        <color rgb="FFB2B2B2"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FFB2B2B2"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top style="thin">
-        <color theme="4"/>
-      </top>
-      <bottom style="double">
-        <color theme="4"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="medium">
-        <color theme="4" tint="0.499984740745262"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color rgb="FF7F7F7F"/>
-      </left>
-      <right style="thin">
-        <color rgb="FF7F7F7F"/>
-      </right>
-      <top style="thin">
-        <color rgb="FF7F7F7F"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FF7F7F7F"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="double">
-        <color rgb="FFFF8001"/>
-      </bottom>
-      <diagonal/>
-    </border>
   </borders>
-  <cellStyleXfs count="49">
+  <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="42" fontId="6" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="22" borderId="7" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="44" fontId="6" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="41" fontId="6" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="43" fontId="6" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="9" fontId="6" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="14" borderId="4" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="6" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="13" borderId="3" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="13" borderId="7" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="4" borderId="1" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="5" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
@@ -1066,58 +495,16 @@
       <alignment horizontal="right"/>
     </xf>
   </cellXfs>
-  <cellStyles count="49">
-    <cellStyle name="常规" xfId="0" builtinId="0"/>
-    <cellStyle name="货币[0]" xfId="1" builtinId="7"/>
-    <cellStyle name="20% - 强调文字颜色 3" xfId="2" builtinId="38"/>
-    <cellStyle name="输入" xfId="3" builtinId="20"/>
-    <cellStyle name="货币" xfId="4" builtinId="4"/>
-    <cellStyle name="千位分隔[0]" xfId="5" builtinId="6"/>
-    <cellStyle name="40% - 强调文字颜色 3" xfId="6" builtinId="39"/>
-    <cellStyle name="差" xfId="7" builtinId="27"/>
-    <cellStyle name="千位分隔" xfId="8" builtinId="3"/>
-    <cellStyle name="60% - 强调文字颜色 3" xfId="9" builtinId="40"/>
-    <cellStyle name="超链接" xfId="10" builtinId="8"/>
-    <cellStyle name="百分比" xfId="11" builtinId="5"/>
-    <cellStyle name="已访问的超链接" xfId="12" builtinId="9"/>
-    <cellStyle name="注释" xfId="13" builtinId="10"/>
-    <cellStyle name="60% - 强调文字颜色 2" xfId="14" builtinId="36"/>
-    <cellStyle name="标题 4" xfId="15" builtinId="19"/>
-    <cellStyle name="警告文本" xfId="16" builtinId="11"/>
-    <cellStyle name="标题" xfId="17" builtinId="15"/>
-    <cellStyle name="解释性文本" xfId="18" builtinId="53"/>
-    <cellStyle name="标题 1" xfId="19" builtinId="16"/>
-    <cellStyle name="标题 2" xfId="20" builtinId="17"/>
-    <cellStyle name="60% - 强调文字颜色 1" xfId="21" builtinId="32"/>
-    <cellStyle name="标题 3" xfId="22" builtinId="18"/>
-    <cellStyle name="60% - 强调文字颜色 4" xfId="23" builtinId="44"/>
-    <cellStyle name="输出" xfId="24" builtinId="21"/>
-    <cellStyle name="计算" xfId="25" builtinId="22"/>
-    <cellStyle name="检查单元格" xfId="26" builtinId="23"/>
-    <cellStyle name="20% - 强调文字颜色 6" xfId="27" builtinId="50"/>
-    <cellStyle name="强调文字颜色 2" xfId="28" builtinId="33"/>
-    <cellStyle name="链接单元格" xfId="29" builtinId="24"/>
-    <cellStyle name="汇总" xfId="30" builtinId="25"/>
-    <cellStyle name="好" xfId="31" builtinId="26"/>
-    <cellStyle name="适中" xfId="32" builtinId="28"/>
-    <cellStyle name="20% - 强调文字颜色 5" xfId="33" builtinId="46"/>
-    <cellStyle name="强调文字颜色 1" xfId="34" builtinId="29"/>
-    <cellStyle name="20% - 强调文字颜色 1" xfId="35" builtinId="30"/>
-    <cellStyle name="40% - 强调文字颜色 1" xfId="36" builtinId="31"/>
-    <cellStyle name="20% - 强调文字颜色 2" xfId="37" builtinId="34"/>
-    <cellStyle name="40% - 强调文字颜色 2" xfId="38" builtinId="35"/>
-    <cellStyle name="强调文字颜色 3" xfId="39" builtinId="37"/>
-    <cellStyle name="强调文字颜色 4" xfId="40" builtinId="41"/>
-    <cellStyle name="20% - 强调文字颜色 4" xfId="41" builtinId="42"/>
-    <cellStyle name="40% - 强调文字颜色 4" xfId="42" builtinId="43"/>
-    <cellStyle name="强调文字颜色 5" xfId="43" builtinId="45"/>
-    <cellStyle name="40% - 强调文字颜色 5" xfId="44" builtinId="47"/>
-    <cellStyle name="60% - 强调文字颜色 5" xfId="45" builtinId="48"/>
-    <cellStyle name="强调文字颜色 6" xfId="46" builtinId="49"/>
-    <cellStyle name="40% - 强调文字颜色 6" xfId="47" builtinId="51"/>
-    <cellStyle name="60% - 强调文字颜色 6" xfId="48" builtinId="52"/>
+  <cellStyles count="1">
+    <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
+  <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
+      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+  </extLst>
 </styleSheet>
 </file>
 
@@ -1449,24 +836,24 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-  <sheetPr/>
-  <dimension ref="A1:F23"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:F24"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F31" sqref="F31"/>
+      <selection activeCell="I17" sqref="I17"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9" defaultRowHeight="13.5" outlineLevelCol="5"/>
+  <sheetFormatPr defaultColWidth="9" defaultRowHeight="13.5" x14ac:dyDescent="0.15"/>
   <cols>
     <col min="1" max="1" width="21.625" customWidth="1"/>
     <col min="2" max="2" width="6.5" customWidth="1"/>
     <col min="3" max="3" width="12.75" customWidth="1"/>
     <col min="4" max="4" width="29.375" customWidth="1"/>
     <col min="5" max="5" width="12.625" customWidth="1"/>
+    <col min="6" max="6" width="20.5" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="2:6">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.15">
       <c r="B1" t="s">
         <v>0</v>
       </c>
@@ -1483,7 +870,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="2" spans="1:3">
+    <row r="2" spans="1:6" x14ac:dyDescent="0.15">
       <c r="A2" t="s">
         <v>5</v>
       </c>
@@ -1492,7 +879,7 @@
       </c>
       <c r="C2" s="3"/>
     </row>
-    <row r="3" spans="2:4">
+    <row r="3" spans="1:6" x14ac:dyDescent="0.15">
       <c r="B3" s="3"/>
       <c r="C3" s="3" t="s">
         <v>6</v>
@@ -1501,13 +888,13 @@
         <v>7</v>
       </c>
     </row>
-    <row r="4" spans="2:3">
+    <row r="4" spans="1:6" x14ac:dyDescent="0.15">
       <c r="B4" s="3"/>
       <c r="C4" s="3" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="5" spans="1:3">
+    <row r="5" spans="1:6" x14ac:dyDescent="0.15">
       <c r="A5" t="s">
         <v>9</v>
       </c>
@@ -1516,7 +903,7 @@
       </c>
       <c r="C5" s="3"/>
     </row>
-    <row r="6" spans="1:3">
+    <row r="6" spans="1:6" x14ac:dyDescent="0.15">
       <c r="A6" t="s">
         <v>10</v>
       </c>
@@ -1525,7 +912,7 @@
       </c>
       <c r="C6" s="3"/>
     </row>
-    <row r="7" spans="1:3">
+    <row r="7" spans="1:6" x14ac:dyDescent="0.15">
       <c r="A7" t="s">
         <v>11</v>
       </c>
@@ -1534,7 +921,7 @@
       </c>
       <c r="C7" s="3"/>
     </row>
-    <row r="8" spans="1:3">
+    <row r="8" spans="1:6" x14ac:dyDescent="0.15">
       <c r="A8" t="s">
         <v>12</v>
       </c>
@@ -1543,7 +930,7 @@
       </c>
       <c r="C8" s="3"/>
     </row>
-    <row r="9" spans="1:3">
+    <row r="9" spans="1:6" x14ac:dyDescent="0.15">
       <c r="A9" t="s">
         <v>13</v>
       </c>
@@ -1552,7 +939,7 @@
       </c>
       <c r="C9" s="3"/>
     </row>
-    <row r="10" spans="2:4">
+    <row r="10" spans="1:6" x14ac:dyDescent="0.15">
       <c r="B10" s="3"/>
       <c r="C10" s="3" t="s">
         <v>14</v>
@@ -1561,7 +948,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="11" spans="2:4">
+    <row r="11" spans="1:6" x14ac:dyDescent="0.15">
       <c r="B11" s="3"/>
       <c r="C11" s="3" t="s">
         <v>16</v>
@@ -1570,7 +957,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="12" spans="2:6">
+    <row r="12" spans="1:6" x14ac:dyDescent="0.15">
       <c r="B12" s="3"/>
       <c r="C12" s="3"/>
       <c r="E12" t="s">
@@ -1580,7 +967,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="13" spans="2:4">
+    <row r="13" spans="1:6" x14ac:dyDescent="0.15">
       <c r="B13" s="3"/>
       <c r="C13" t="s">
         <v>20</v>
@@ -1589,7 +976,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="14" spans="2:6">
+    <row r="14" spans="1:6" x14ac:dyDescent="0.15">
       <c r="B14" s="3"/>
       <c r="E14" t="s">
         <v>22</v>
@@ -1598,7 +985,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="15" spans="2:6">
+    <row r="15" spans="1:6" x14ac:dyDescent="0.15">
       <c r="B15" s="3"/>
       <c r="E15" t="s">
         <v>24</v>
@@ -1607,7 +994,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="16" spans="2:6">
+    <row r="16" spans="1:6" x14ac:dyDescent="0.15">
       <c r="B16" s="3"/>
       <c r="E16" s="3" t="s">
         <v>26</v>
@@ -1616,7 +1003,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="17" spans="2:6">
+    <row r="17" spans="1:6" x14ac:dyDescent="0.15">
       <c r="B17" s="3"/>
       <c r="E17" s="3" t="s">
         <v>28</v>
@@ -1625,108 +1012,113 @@
         <v>29</v>
       </c>
     </row>
-    <row r="18" spans="2:6">
+    <row r="18" spans="1:6" x14ac:dyDescent="0.15">
       <c r="B18" s="3"/>
       <c r="E18" s="3" t="s">
-        <v>30</v>
+        <v>39</v>
       </c>
       <c r="F18" t="s">
-        <v>31</v>
-      </c>
-    </row>
-    <row r="19" spans="2:6">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="19" spans="1:6" x14ac:dyDescent="0.15">
       <c r="B19" s="3"/>
       <c r="E19" s="3" t="s">
+        <v>30</v>
+      </c>
+      <c r="F19" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="20" spans="1:6" x14ac:dyDescent="0.15">
+      <c r="B20" s="3"/>
+      <c r="E20" s="3" t="s">
         <v>32</v>
       </c>
-      <c r="F19" t="s">
+      <c r="F20" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="21" spans="1:6" x14ac:dyDescent="0.15">
+      <c r="B21" s="3"/>
+      <c r="E21" s="3"/>
+    </row>
+    <row r="22" spans="1:6" x14ac:dyDescent="0.15">
+      <c r="B22" s="3"/>
+      <c r="E22" s="4" t="s">
         <v>33</v>
       </c>
-    </row>
-    <row r="20" spans="2:5">
-      <c r="B20" s="3"/>
-      <c r="E20" s="3"/>
-    </row>
-    <row r="21" spans="2:6">
-      <c r="B21" s="3"/>
-      <c r="E21" s="4" t="s">
+      <c r="F22" t="s">
         <v>34</v>
       </c>
-      <c r="F21" t="s">
+    </row>
+    <row r="23" spans="1:6" x14ac:dyDescent="0.15">
+      <c r="A23" t="s">
         <v>35</v>
       </c>
-    </row>
-    <row r="22" spans="1:3">
-      <c r="A22" t="s">
+      <c r="B23" s="3">
+        <v>70000</v>
+      </c>
+      <c r="C23" s="3"/>
+    </row>
+    <row r="24" spans="1:6" s="1" customFormat="1" x14ac:dyDescent="0.15">
+      <c r="A24" s="1" t="s">
         <v>36</v>
       </c>
-      <c r="B22" s="3">
-        <v>70000</v>
-      </c>
-      <c r="C22" s="3"/>
-    </row>
-    <row r="23" s="1" customFormat="1" spans="1:3">
-      <c r="A23" s="1" t="s">
-        <v>37</v>
-      </c>
-      <c r="B23" s="5">
+      <c r="B24" s="5">
         <v>80000</v>
       </c>
-      <c r="C23" s="5"/>
+      <c r="C24" s="5"/>
     </row>
   </sheetData>
-  <pageMargins left="0.699305555555556" right="0.699305555555556" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <phoneticPr fontId="2" type="noConversion"/>
+  <pageMargins left="0.69930555555555596" right="0.69930555555555596" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait"/>
-  <headerFooter/>
-  <legacyDrawing r:id="rId2"/>
+  <legacyDrawing r:id="rId1"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-  <sheetPr/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A2:B3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="C9" sqref="C9"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9" defaultRowHeight="13.5" outlineLevelRow="2" outlineLevelCol="1"/>
+  <sheetFormatPr defaultColWidth="9" defaultRowHeight="13.5" x14ac:dyDescent="0.15"/>
   <sheetData>
-    <row r="2" spans="1:2">
+    <row r="2" spans="1:2" x14ac:dyDescent="0.15">
       <c r="A2" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="B2">
         <v>50000</v>
       </c>
     </row>
-    <row r="3" spans="1:2">
+    <row r="3" spans="1:2" x14ac:dyDescent="0.15">
       <c r="A3" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="B3">
         <v>50100</v>
       </c>
     </row>
   </sheetData>
-  <pageMargins left="0.699305555555556" right="0.699305555555556" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <headerFooter/>
+  <phoneticPr fontId="2" type="noConversion"/>
+  <pageMargins left="0.69930555555555596" right="0.69930555555555596" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-  <sheetPr/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A1" sqref="A1"/>
-    </sheetView>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9" defaultRowHeight="13.5"/>
+  <sheetFormatPr defaultColWidth="9" defaultRowHeight="13.5" x14ac:dyDescent="0.15"/>
   <sheetData/>
-  <pageMargins left="0.699305555555556" right="0.699305555555556" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <headerFooter/>
+  <phoneticPr fontId="2" type="noConversion"/>
+  <pageMargins left="0.69930555555555596" right="0.69930555555555596" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
2017-03-01: 1. AC empty show all items; 2. billType in bill not show top recorder;
</commit_message>
<xml_diff>
--- a/doc/error_code_range.xlsx
+++ b/doc/error_code_range.xlsx
@@ -1,10 +1,10 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
+  <fileVersion appName="xl" lastEdited="3" lowestEdited="5" rupBuild="9302"/>
   <workbookPr/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="60" windowWidth="28695" windowHeight="12990"/>
+    <workbookView windowWidth="28695" windowHeight="13050"/>
   </bookViews>
   <sheets>
     <sheet name="all" sheetId="1" r:id="rId1"/>
@@ -30,16 +30,8 @@
             <rFont val="宋体"/>
             <charset val="134"/>
           </rPr>
-          <t xml:space="preserve">zw:
-</t>
-        </r>
-        <r>
-          <rPr>
-            <sz val="9"/>
-            <rFont val="宋体"/>
-            <charset val="134"/>
-          </rPr>
-          <t>对浏览器传入的值的定义</t>
+          <t>zw:
+对浏览器传入的值的定义</t>
         </r>
       </text>
     </comment>
@@ -52,15 +44,7 @@
             <charset val="134"/>
           </rPr>
           <t xml:space="preserve">zw:
-</t>
-        </r>
-        <r>
-          <rPr>
-            <sz val="9"/>
-            <rFont val="宋体"/>
-            <charset val="134"/>
-          </rPr>
-          <t xml:space="preserve">对要存入mongodb的数据（一般是从浏览器传入）的数值，用mongoose的validator进行验证
+对要存入mongodb的数据（一般是从浏览器传入）的数值，用mongoose的validator进行验证
 </t>
         </r>
       </text>
@@ -74,15 +58,7 @@
             <charset val="134"/>
           </rPr>
           <t xml:space="preserve">zw:
-</t>
-        </r>
-        <r>
-          <rPr>
-            <sz val="9"/>
-            <rFont val="宋体"/>
-            <charset val="134"/>
-          </rPr>
-          <t xml:space="preserve">在对数据进行操作（CRUD等）发生的错误
+在对数据进行操作（CRUD等）发生的错误
 </t>
         </r>
       </text>
@@ -96,15 +72,7 @@
             <charset val="134"/>
           </rPr>
           <t xml:space="preserve">zw:
-</t>
-        </r>
-        <r>
-          <rPr>
-            <sz val="9"/>
-            <rFont val="宋体"/>
-            <charset val="134"/>
-          </rPr>
-          <t xml:space="preserve">在对数据进行操作（CRUD等）发生的错误
+在对数据进行操作（CRUD等）发生的错误
 </t>
         </r>
       </text>
@@ -117,16 +85,8 @@
             <rFont val="宋体"/>
             <charset val="134"/>
           </rPr>
-          <t xml:space="preserve">zw:
-</t>
-        </r>
-        <r>
-          <rPr>
-            <sz val="9"/>
-            <rFont val="宋体"/>
-            <charset val="134"/>
-          </rPr>
-          <t>运行node代码时发生的错误。除了包含web page的error code，也包含assist的error code</t>
+          <t>zw:
+运行node代码时发生的错误。除了包含web page的error code，也包含assist的error code</t>
         </r>
       </text>
     </comment>
@@ -138,16 +98,8 @@
             <rFont val="宋体"/>
             <charset val="134"/>
           </rPr>
-          <t xml:space="preserve">ZHANG Wei AG:
-</t>
-        </r>
-        <r>
-          <rPr>
-            <sz val="9"/>
-            <rFont val="宋体"/>
-            <charset val="134"/>
-          </rPr>
-          <t>server端上传文件处理，直接定义在类文件，而不是单独error code文件</t>
+          <t>ZHANG Wei AG:
+server端上传文件处理，直接定义在类文件，而不是单独error code文件</t>
         </r>
       </text>
     </comment>
@@ -159,16 +111,8 @@
             <rFont val="宋体"/>
             <charset val="134"/>
           </rPr>
-          <t xml:space="preserve">ZHANG Wei AG:
-</t>
-        </r>
-        <r>
-          <rPr>
-            <sz val="9"/>
-            <rFont val="宋体"/>
-            <charset val="134"/>
-          </rPr>
-          <t>使用gm对image进行操作，是个类</t>
+          <t>ZHANG Wei AG:
+使用gm对image进行操作，是个类</t>
         </r>
       </text>
     </comment>
@@ -193,16 +137,8 @@
             <rFont val="宋体"/>
             <charset val="134"/>
           </rPr>
-          <t xml:space="preserve">ZHANG Wei AG:
-</t>
-        </r>
-        <r>
-          <rPr>
-            <sz val="9"/>
-            <rFont val="宋体"/>
-            <charset val="134"/>
-          </rPr>
-          <t>虽然在misc中，但是是个大函数，所以有单独的error code范围</t>
+          <t>ZHANG Wei AG:
+虽然在misc中，但是是个大函数，所以有单独的error code范围</t>
         </r>
       </text>
     </comment>
@@ -214,16 +150,8 @@
             <rFont val="宋体"/>
             <charset val="134"/>
           </rPr>
-          <t xml:space="preserve">zw:
-</t>
-        </r>
-        <r>
-          <rPr>
-            <sz val="9"/>
-            <rFont val="宋体"/>
-            <charset val="134"/>
-          </rPr>
-          <t>全局配置以及对应的错误</t>
+          <t>zw:
+全局配置以及对应的错误</t>
         </r>
       </text>
     </comment>
@@ -235,16 +163,8 @@
             <rFont val="宋体"/>
             <charset val="134"/>
           </rPr>
-          <t xml:space="preserve">zw:
-</t>
-        </r>
-        <r>
-          <rPr>
-            <sz val="9"/>
-            <rFont val="宋体"/>
-            <charset val="134"/>
-          </rPr>
-          <t>单独定义在image中。使用gm对image操作是发生的错误</t>
+          <t>zw:
+单独定义在image中。使用gm对image操作是发生的错误</t>
         </r>
       </text>
     </comment>
@@ -253,7 +173,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="42" uniqueCount="42">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="43">
   <si>
     <t>rc</t>
   </si>
@@ -313,7 +233,10 @@
     <t>general for valid function</t>
   </si>
   <si>
-    <t>other</t>
+    <t>19000~19999</t>
+  </si>
+  <si>
+    <t>临时error code。为那些没有在inputRule中定义（db中没有对应字段）的字段设置</t>
   </si>
   <si>
     <t>mongo_validate</t>
@@ -379,6 +302,12 @@
     <t>gmImage</t>
   </si>
   <si>
+    <t>69500-69599</t>
+  </si>
+  <si>
+    <t>validateInputSearch</t>
+  </si>
+  <si>
     <t>69700-69799</t>
   </si>
   <si>
@@ -386,6 +315,9 @@
   </si>
   <si>
     <t>69800-69899</t>
+  </si>
+  <si>
+    <t>validateInputRule</t>
   </si>
   <si>
     <r>
@@ -422,24 +354,18 @@
   <si>
     <t>uploadDefine</t>
   </si>
-  <si>
-    <t>69500-69599</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>validateInputRule</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>validateInputSearch</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="3" x14ac:knownFonts="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <numFmts count="4">
+    <numFmt numFmtId="44" formatCode="_ &quot;￥&quot;* #,##0.00_ ;_ &quot;￥&quot;* \-#,##0.00_ ;_ &quot;￥&quot;* &quot;-&quot;??_ ;_ @_ "/>
+    <numFmt numFmtId="41" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
+    <numFmt numFmtId="43" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
+    <numFmt numFmtId="42" formatCode="_ &quot;￥&quot;* #,##0_ ;_ &quot;￥&quot;* \-#,##0_ ;_ &quot;￥&quot;* &quot;-&quot;_ ;_ @_ "/>
+  </numFmts>
+  <fonts count="22">
     <font>
       <sz val="11"/>
       <color indexed="8"/>
@@ -454,20 +380,352 @@
       <charset val="134"/>
     </font>
     <font>
-      <sz val="9"/>
+      <sz val="11"/>
+      <color rgb="FFFF0000"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
       <name val="宋体"/>
       <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="18"/>
+      <color theme="3"/>
+      <name val="宋体"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color rgb="FF0000FF"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <i/>
+      <sz val="11"/>
+      <color rgb="FF7F7F7F"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="3"/>
+      <name val="宋体"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF9C0006"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="0"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF9C6500"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF3F3F76"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF006100"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color rgb="FF800080"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFA7D00"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FF3F3F3F"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="15"/>
+      <color theme="3"/>
+      <name val="宋体"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FFFFFFFF"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="13"/>
+      <color theme="3"/>
+      <name val="宋体"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FFFA7D00"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="2">
+  <fills count="33">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFFCC"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFC7CE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFEB9C"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFCC99"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFC6EFCE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFF2F2F2"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFA5A5A5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="1">
+  <borders count="9">
     <border>
       <left/>
       <right/>
@@ -475,9 +733,251 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color rgb="FFB2B2B2"/>
+      </left>
+      <right style="thin">
+        <color rgb="FFB2B2B2"/>
+      </right>
+      <top style="thin">
+        <color rgb="FFB2B2B2"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FFB2B2B2"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FF7F7F7F"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF7F7F7F"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF7F7F7F"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF7F7F7F"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="double">
+        <color rgb="FFFF8001"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FF3F3F3F"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF3F3F3F"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF3F3F3F"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF3F3F3F"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color theme="4"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="double">
+        <color rgb="FF3F3F3F"/>
+      </left>
+      <right style="double">
+        <color rgb="FF3F3F3F"/>
+      </right>
+      <top style="double">
+        <color rgb="FF3F3F3F"/>
+      </top>
+      <bottom style="double">
+        <color rgb="FF3F3F3F"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color theme="4"/>
+      </top>
+      <bottom style="double">
+        <color theme="4"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color theme="4" tint="0.499984740745262"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="49">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="42" fontId="3" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="11" borderId="2" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="44" fontId="3" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="41" fontId="3" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="43" fontId="3" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="9" fontId="3" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="1" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="5" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="5" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="21" borderId="4" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="21" borderId="2" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="26" borderId="6" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="7" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
@@ -495,16 +995,58 @@
       <alignment horizontal="right"/>
     </xf>
   </cellXfs>
-  <cellStyles count="1">
-    <cellStyle name="Normal" xfId="0" builtinId="0"/>
+  <cellStyles count="49">
+    <cellStyle name="常规" xfId="0" builtinId="0"/>
+    <cellStyle name="货币[0]" xfId="1" builtinId="7"/>
+    <cellStyle name="20% - 强调文字颜色 3" xfId="2" builtinId="38"/>
+    <cellStyle name="输入" xfId="3" builtinId="20"/>
+    <cellStyle name="货币" xfId="4" builtinId="4"/>
+    <cellStyle name="千位分隔[0]" xfId="5" builtinId="6"/>
+    <cellStyle name="40% - 强调文字颜色 3" xfId="6" builtinId="39"/>
+    <cellStyle name="差" xfId="7" builtinId="27"/>
+    <cellStyle name="千位分隔" xfId="8" builtinId="3"/>
+    <cellStyle name="60% - 强调文字颜色 3" xfId="9" builtinId="40"/>
+    <cellStyle name="超链接" xfId="10" builtinId="8"/>
+    <cellStyle name="百分比" xfId="11" builtinId="5"/>
+    <cellStyle name="已访问的超链接" xfId="12" builtinId="9"/>
+    <cellStyle name="注释" xfId="13" builtinId="10"/>
+    <cellStyle name="60% - 强调文字颜色 2" xfId="14" builtinId="36"/>
+    <cellStyle name="标题 4" xfId="15" builtinId="19"/>
+    <cellStyle name="警告文本" xfId="16" builtinId="11"/>
+    <cellStyle name="标题" xfId="17" builtinId="15"/>
+    <cellStyle name="解释性文本" xfId="18" builtinId="53"/>
+    <cellStyle name="标题 1" xfId="19" builtinId="16"/>
+    <cellStyle name="标题 2" xfId="20" builtinId="17"/>
+    <cellStyle name="60% - 强调文字颜色 1" xfId="21" builtinId="32"/>
+    <cellStyle name="标题 3" xfId="22" builtinId="18"/>
+    <cellStyle name="60% - 强调文字颜色 4" xfId="23" builtinId="44"/>
+    <cellStyle name="输出" xfId="24" builtinId="21"/>
+    <cellStyle name="计算" xfId="25" builtinId="22"/>
+    <cellStyle name="检查单元格" xfId="26" builtinId="23"/>
+    <cellStyle name="20% - 强调文字颜色 6" xfId="27" builtinId="50"/>
+    <cellStyle name="强调文字颜色 2" xfId="28" builtinId="33"/>
+    <cellStyle name="链接单元格" xfId="29" builtinId="24"/>
+    <cellStyle name="汇总" xfId="30" builtinId="25"/>
+    <cellStyle name="好" xfId="31" builtinId="26"/>
+    <cellStyle name="适中" xfId="32" builtinId="28"/>
+    <cellStyle name="20% - 强调文字颜色 5" xfId="33" builtinId="46"/>
+    <cellStyle name="强调文字颜色 1" xfId="34" builtinId="29"/>
+    <cellStyle name="20% - 强调文字颜色 1" xfId="35" builtinId="30"/>
+    <cellStyle name="40% - 强调文字颜色 1" xfId="36" builtinId="31"/>
+    <cellStyle name="20% - 强调文字颜色 2" xfId="37" builtinId="34"/>
+    <cellStyle name="40% - 强调文字颜色 2" xfId="38" builtinId="35"/>
+    <cellStyle name="强调文字颜色 3" xfId="39" builtinId="37"/>
+    <cellStyle name="强调文字颜色 4" xfId="40" builtinId="41"/>
+    <cellStyle name="20% - 强调文字颜色 4" xfId="41" builtinId="42"/>
+    <cellStyle name="40% - 强调文字颜色 4" xfId="42" builtinId="43"/>
+    <cellStyle name="强调文字颜色 5" xfId="43" builtinId="45"/>
+    <cellStyle name="40% - 强调文字颜色 5" xfId="44" builtinId="47"/>
+    <cellStyle name="60% - 强调文字颜色 5" xfId="45" builtinId="48"/>
+    <cellStyle name="强调文字颜色 6" xfId="46" builtinId="49"/>
+    <cellStyle name="40% - 强调文字颜色 6" xfId="47" builtinId="51"/>
+    <cellStyle name="60% - 强调文字颜色 6" xfId="48" builtinId="52"/>
   </cellStyles>
-  <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2"/>
-  <extLst>
-    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
-      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
-    </ext>
-  </extLst>
 </styleSheet>
 </file>
 
@@ -836,24 +1378,25 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+  <sheetPr/>
   <dimension ref="A1:F24"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I17" sqref="I17"/>
+      <selection activeCell="D4" sqref="D4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9" defaultRowHeight="13.5" x14ac:dyDescent="0.15"/>
+  <sheetFormatPr defaultColWidth="9" defaultRowHeight="13.5" outlineLevelCol="5"/>
   <cols>
     <col min="1" max="1" width="21.625" customWidth="1"/>
     <col min="2" max="2" width="6.5" customWidth="1"/>
     <col min="3" max="3" width="12.75" customWidth="1"/>
     <col min="4" max="4" width="29.375" customWidth="1"/>
     <col min="5" max="5" width="12.625" customWidth="1"/>
-    <col min="6" max="6" width="20.5" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="20.5" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.15">
+    <row r="1" spans="2:6">
       <c r="B1" t="s">
         <v>0</v>
       </c>
@@ -870,7 +1413,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.15">
+    <row r="2" spans="1:3">
       <c r="A2" t="s">
         <v>5</v>
       </c>
@@ -879,7 +1422,7 @@
       </c>
       <c r="C2" s="3"/>
     </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.15">
+    <row r="3" spans="2:4">
       <c r="B3" s="3"/>
       <c r="C3" s="3" t="s">
         <v>6</v>
@@ -888,182 +1431,185 @@
         <v>7</v>
       </c>
     </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.15">
+    <row r="4" spans="2:4">
       <c r="B4" s="3"/>
       <c r="C4" s="3" t="s">
         <v>8</v>
       </c>
-    </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.15">
+      <c r="D4" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3">
       <c r="A5" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="B5" s="3">
         <v>20000</v>
       </c>
       <c r="C5" s="3"/>
     </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.15">
+    <row r="6" spans="1:3">
       <c r="A6" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="B6" s="3">
         <v>30000</v>
       </c>
       <c r="C6" s="3"/>
     </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.15">
+    <row r="7" spans="1:3">
       <c r="A7" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="B7" s="3">
         <v>40000</v>
       </c>
       <c r="C7" s="3"/>
     </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.15">
+    <row r="8" spans="1:3">
       <c r="A8" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="B8" s="3">
         <v>50000</v>
       </c>
       <c r="C8" s="3"/>
     </row>
-    <row r="9" spans="1:6" x14ac:dyDescent="0.15">
+    <row r="9" spans="1:3">
       <c r="A9" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="B9" s="3">
         <v>60000</v>
       </c>
       <c r="C9" s="3"/>
     </row>
-    <row r="10" spans="1:6" x14ac:dyDescent="0.15">
+    <row r="10" spans="2:4">
       <c r="B10" s="3"/>
       <c r="C10" s="3" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="D10" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="11" spans="1:6" x14ac:dyDescent="0.15">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="11" spans="2:4">
       <c r="B11" s="3"/>
       <c r="C11" s="3" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="D11" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="12" spans="1:6" x14ac:dyDescent="0.15">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="12" spans="2:6">
       <c r="B12" s="3"/>
       <c r="C12" s="3"/>
       <c r="E12" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="F12" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="13" spans="1:6" x14ac:dyDescent="0.15">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="13" spans="2:4">
       <c r="B13" s="3"/>
       <c r="C13" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="D13" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="14" spans="1:6" x14ac:dyDescent="0.15">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="14" spans="2:6">
       <c r="B14" s="3"/>
       <c r="E14" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="F14" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="15" spans="1:6" x14ac:dyDescent="0.15">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="15" spans="2:6">
       <c r="B15" s="3"/>
       <c r="E15" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="F15" t="s">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="16" spans="1:6" x14ac:dyDescent="0.15">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="16" spans="2:6">
       <c r="B16" s="3"/>
       <c r="E16" s="3" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="F16" s="2" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="17" spans="1:6" x14ac:dyDescent="0.15">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="17" spans="2:6">
       <c r="B17" s="3"/>
       <c r="E17" s="3" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="F17" t="s">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="18" spans="1:6" x14ac:dyDescent="0.15">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="18" spans="2:6">
       <c r="B18" s="3"/>
       <c r="E18" s="3" t="s">
-        <v>39</v>
+        <v>31</v>
       </c>
       <c r="F18" t="s">
-        <v>41</v>
-      </c>
-    </row>
-    <row r="19" spans="1:6" x14ac:dyDescent="0.15">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="19" spans="2:6">
       <c r="B19" s="3"/>
       <c r="E19" s="3" t="s">
-        <v>30</v>
+        <v>33</v>
       </c>
       <c r="F19" t="s">
-        <v>31</v>
-      </c>
-    </row>
-    <row r="20" spans="1:6" x14ac:dyDescent="0.15">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="20" spans="2:6">
       <c r="B20" s="3"/>
       <c r="E20" s="3" t="s">
-        <v>32</v>
+        <v>35</v>
       </c>
       <c r="F20" t="s">
-        <v>40</v>
-      </c>
-    </row>
-    <row r="21" spans="1:6" x14ac:dyDescent="0.15">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="21" spans="2:5">
       <c r="B21" s="3"/>
       <c r="E21" s="3"/>
     </row>
-    <row r="22" spans="1:6" x14ac:dyDescent="0.15">
+    <row r="22" spans="2:6">
       <c r="B22" s="3"/>
       <c r="E22" s="4" t="s">
-        <v>33</v>
+        <v>37</v>
       </c>
       <c r="F22" t="s">
-        <v>34</v>
-      </c>
-    </row>
-    <row r="23" spans="1:6" x14ac:dyDescent="0.15">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="23" spans="1:3">
       <c r="A23" t="s">
-        <v>35</v>
+        <v>39</v>
       </c>
       <c r="B23" s="3">
         <v>70000</v>
       </c>
       <c r="C23" s="3"/>
     </row>
-    <row r="24" spans="1:6" s="1" customFormat="1" x14ac:dyDescent="0.15">
+    <row r="24" s="1" customFormat="1" spans="1:3">
       <c r="A24" s="1" t="s">
-        <v>36</v>
+        <v>40</v>
       </c>
       <c r="B24" s="5">
         <v>80000</v>
@@ -1071,54 +1617,58 @@
       <c r="C24" s="5"/>
     </row>
   </sheetData>
-  <phoneticPr fontId="2" type="noConversion"/>
-  <pageMargins left="0.69930555555555596" right="0.69930555555555596" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageMargins left="0.699305555555556" right="0.699305555555556" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait"/>
-  <legacyDrawing r:id="rId1"/>
+  <headerFooter/>
+  <legacyDrawing r:id="rId2"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+  <sheetPr/>
   <dimension ref="A2:B3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="C9" sqref="C9"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9" defaultRowHeight="13.5" x14ac:dyDescent="0.15"/>
+  <sheetFormatPr defaultColWidth="9" defaultRowHeight="13.5" outlineLevelRow="2" outlineLevelCol="1"/>
   <sheetData>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.15">
+    <row r="2" spans="1:2">
       <c r="A2" t="s">
-        <v>37</v>
+        <v>41</v>
       </c>
       <c r="B2">
         <v>50000</v>
       </c>
     </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.15">
+    <row r="3" spans="1:2">
       <c r="A3" t="s">
-        <v>38</v>
+        <v>42</v>
       </c>
       <c r="B3">
         <v>50100</v>
       </c>
     </row>
   </sheetData>
-  <phoneticPr fontId="2" type="noConversion"/>
-  <pageMargins left="0.69930555555555596" right="0.69930555555555596" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageMargins left="0.699305555555556" right="0.699305555555556" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <headerFooter/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+  <sheetPr/>
   <dimension ref="A1"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9" defaultRowHeight="13.5" x14ac:dyDescent="0.15"/>
+  <sheetFormatPr defaultColWidth="9" defaultRowHeight="13.5"/>
   <sheetData/>
-  <phoneticPr fontId="2" type="noConversion"/>
-  <pageMargins left="0.69930555555555596" right="0.69930555555555596" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageMargins left="0.699305555555556" right="0.699305555555556" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <headerFooter/>
 </worksheet>
 </file>
</xml_diff>